<commit_message>
Update for next week.
</commit_message>
<xml_diff>
--- a/October 2014.xlsx
+++ b/October 2014.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t>Nazwa</t>
   </si>
@@ -48,18 +48,12 @@
     <t>Termin wykonania najbliższego etapu</t>
   </si>
   <si>
-    <t>23.09.2014</t>
-  </si>
-  <si>
     <t>Systemy Uczące</t>
   </si>
   <si>
     <t>Cykliczna laborka z Data Mining</t>
   </si>
   <si>
-    <t>20.09.2014</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>Dopasować temat</t>
   </si>
   <si>
-    <t>21.09.2014</t>
-  </si>
-  <si>
     <t>Inżynieria języka</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>Dobrać temat, doczytać w sym eval</t>
   </si>
   <si>
-    <t>22.09.2014</t>
-  </si>
-  <si>
     <t>15.01.2014</t>
   </si>
   <si>
@@ -325,6 +313,39 @@
   </si>
   <si>
     <t>Stolarz?</t>
+  </si>
+  <si>
+    <t>Bazy danych</t>
+  </si>
+  <si>
+    <t>Praca magisterska</t>
+  </si>
+  <si>
+    <t>MGR</t>
+  </si>
+  <si>
+    <t>23.10.2014</t>
+  </si>
+  <si>
+    <t>20.10.2014</t>
+  </si>
+  <si>
+    <t>21.10.2014</t>
+  </si>
+  <si>
+    <t>22.10.2014</t>
+  </si>
+  <si>
+    <t>dokończ DI 1h</t>
+  </si>
+  <si>
+    <t>PF - 1,5h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SU </t>
+  </si>
+  <si>
+    <t>Mail MGR</t>
   </si>
 </sst>
 </file>
@@ -861,9 +882,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -873,87 +891,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
@@ -962,6 +908,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -973,6 +973,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1281,7 +1302,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,33 +1315,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="A1" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>57</v>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1334,7 +1355,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,7 +1383,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1374,114 +1395,118 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>60</v>
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>61</v>
+        <v>12</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>64</v>
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>65</v>
+      <c r="F9" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>66</v>
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="6" t="s">
-        <v>62</v>
+      <c r="F11" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1553,7 +1578,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1586,7 @@
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
@@ -1572,379 +1597,389 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38"/>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="19"/>
+      <c r="I3" s="36"/>
       <c r="L3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" s="22"/>
+        <v>68</v>
+      </c>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="51"/>
+      <c r="A4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="26"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="30" t="s">
-        <v>70</v>
+      <c r="D4" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="52" t="s">
-        <v>42</v>
+      <c r="I4" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
-      </c>
-      <c r="M4" s="23"/>
+        <v>69</v>
+      </c>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="31"/>
+      <c r="A5" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="53" t="s">
-        <v>43</v>
+      <c r="I5" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="33"/>
+        <v>80</v>
+      </c>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="31"/>
+      <c r="A6" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="16"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="53" t="s">
-        <v>44</v>
+      <c r="I6" s="28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="31"/>
+      <c r="A7" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="53" t="s">
-        <v>45</v>
+      <c r="I7" s="28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>78</v>
+      <c r="A8" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>74</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="53" t="s">
-        <v>46</v>
+      <c r="I8" s="28" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="27"/>
+      <c r="A9" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="53" t="s">
-        <v>47</v>
+      <c r="I9" s="28" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="26" t="s">
-        <v>79</v>
+      <c r="A10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="39" t="s">
+        <v>75</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="53" t="s">
-        <v>48</v>
+      <c r="I10" s="28" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="27"/>
+      <c r="A11" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="53" t="s">
-        <v>49</v>
+      <c r="I11" s="28" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>80</v>
+      <c r="A12" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="53" t="s">
-        <v>50</v>
+      <c r="I12" s="28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="27"/>
+      <c r="A13" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="53" t="s">
-        <v>76</v>
+      <c r="I13" s="28" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>82</v>
+      <c r="A14" s="24"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>78</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="53" t="s">
-        <v>51</v>
+      <c r="I14" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="53" t="s">
-        <v>52</v>
+      <c r="I15" s="28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="35"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="58"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="53" t="s">
-        <v>53</v>
+      <c r="I16" s="28" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="36"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="53" t="s">
-        <v>81</v>
+      <c r="I17" s="28" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="20" t="s">
-        <v>69</v>
+      <c r="A18" s="24"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="41" t="s">
+        <v>65</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="24" t="s">
-        <v>69</v>
+      <c r="F18" s="55" t="s">
+        <v>65</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="53" t="s">
-        <v>54</v>
+      <c r="I18" s="28" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="21"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="25"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="40" t="s">
-        <v>85</v>
+      <c r="I21" s="46" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="44" t="s">
+      <c r="A22" s="24"/>
+      <c r="B22" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="42"/>
+      <c r="H22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="47"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="1"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="42"/>
+      <c r="I23" s="47"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="56" t="s">
-        <v>92</v>
+      <c r="A24" s="24"/>
+      <c r="B24" s="49" t="s">
+        <v>88</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1952,45 +1987,45 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="42"/>
+      <c r="I24" s="47"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="57"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="42"/>
+      <c r="I25" s="47"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="57"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="42"/>
+      <c r="I26" s="47"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="58"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="42"/>
+      <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="56" t="s">
-        <v>93</v>
+      <c r="A28" s="24"/>
+      <c r="B28" s="49" t="s">
+        <v>89</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1998,18 +2033,18 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="42"/>
+      <c r="I28" s="47"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="43"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>